<commit_message>
Updated for a Server Limited in GCC-H L2
</commit_message>
<xml_diff>
--- a/Ariento Pricing 2025.xlsx
+++ b/Ariento Pricing 2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://arientogroup-my.sharepoint.com/personal/jeffery_robichaux_ariento_com/Documents/Apps/Quote Tool/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://arientogroup-my.sharepoint.com/personal/jeffery_robichaux_ariento_com/Documents/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{1C36343F-1D4C-4388-9958-90A0DD56BDCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1986166-C41C-46D3-9FFA-BCD26539D987}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="8_{1C36343F-1D4C-4388-9958-90A0DD56BDCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44F00462-ADD5-4D3C-9111-C88D55A77B08}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ariento Quote Tool" sheetId="11" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Additional Licenses'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Ariento License Type'!$A$1:$C$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Ariento License Type'!$A$1:$C$63</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Ariento Plans'!$A$1:$A$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Microsoft Licenses'!$A$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Microsoft Seat Licenses'!$A$1:$C$684</definedName>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5764" uniqueCount="1713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5766" uniqueCount="1714">
   <si>
     <t>Plan Name</t>
   </si>
@@ -5189,6 +5189,9 @@
   </si>
   <si>
     <t>Microsoft 365 G5 (GCC Pricing) *Annual Term</t>
+  </si>
+  <si>
+    <t>Turnkey CMMC Level 2 Plan (GCC-High) *Legacy</t>
   </si>
 </sst>
 </file>
@@ -5666,7 +5669,7 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5731,10 +5734,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B55" sqref="A55:C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6340,7 +6343,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>7</v>
+        <v>1713</v>
       </c>
       <c r="B55" t="s">
         <v>18</v>
@@ -6354,54 +6357,54 @@
         <v>7</v>
       </c>
       <c r="B56" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C56" s="9">
-        <v>349</v>
+        <v>999</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B57" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C57" s="9">
-        <v>9</v>
+        <v>349</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B58" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C58" s="9">
-        <v>179</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B59" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C59" s="9">
-        <v>99</v>
+        <v>179</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B60" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C60" s="9">
-        <v>349</v>
+        <v>99</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -6409,27 +6412,38 @@
         <v>6</v>
       </c>
       <c r="B61" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C61" s="9">
-        <v>199</v>
+        <v>349</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B62" t="s">
         <v>15</v>
       </c>
       <c r="C62" s="9">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" t="s">
+        <v>15</v>
+      </c>
+      <c r="C63" s="9">
         <v>249</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C62" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A12:C62">
-      <sortCondition ref="A1:A62"/>
+  <autoFilter ref="A1:C63" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A12:C63">
+      <sortCondition ref="A1:A63"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6440,8 +6454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G684"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:A56"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fixed naming in Ariento Licenses for Commercial
</commit_message>
<xml_diff>
--- a/Ariento Pricing 2025.xlsx
+++ b/Ariento Pricing 2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://arientogroup-my.sharepoint.com/personal/jeffery_robichaux_ariento_com/Documents/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JefferyRobichaux\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="8_{1C36343F-1D4C-4388-9958-90A0DD56BDCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D181DF62-F373-4EBA-8F41-53BA38021AEF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{922B01C3-C890-4F6E-B60A-541624727621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ariento Quote Tool" sheetId="11" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5766" uniqueCount="1713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5766" uniqueCount="1714">
   <si>
     <t>Plan Name</t>
   </si>
@@ -5189,6 +5189,9 @@
   </si>
   <si>
     <t>Microsoft 365 G5 (GCC Pricing) *Annual Term</t>
+  </si>
+  <si>
+    <t>Professional Plan (Commercial)</t>
   </si>
 </sst>
 </file>
@@ -5665,8 +5668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EE40B50-ADD7-4F1C-8302-825C83271F83}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5681,7 +5684,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -5731,10 +5734,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5755,7 +5759,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1679</v>
       </c>
@@ -5766,7 +5770,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1679</v>
       </c>
@@ -5777,7 +5781,7 @@
         <v>4188</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1679</v>
       </c>
@@ -5788,7 +5792,7 @@
         <v>5988</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1680</v>
       </c>
@@ -5799,7 +5803,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1680</v>
       </c>
@@ -5810,7 +5814,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1680</v>
       </c>
@@ -5823,7 +5827,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>1713</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -5832,7 +5836,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -5843,7 +5847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -5854,7 +5858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -5865,7 +5869,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -5876,7 +5880,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -5887,7 +5891,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -5900,7 +5904,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>1713</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
@@ -5909,7 +5913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -5920,7 +5924,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -5931,7 +5935,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -5942,7 +5946,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -5955,7 +5959,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>1</v>
+        <v>1713</v>
       </c>
       <c r="B20" t="s">
         <v>16</v>
@@ -5964,7 +5968,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -5975,7 +5979,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -5986,7 +5990,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -5997,7 +6001,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -6008,7 +6012,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -6019,7 +6023,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -6032,7 +6036,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>1</v>
+        <v>1713</v>
       </c>
       <c r="B27" t="s">
         <v>14</v>
@@ -6041,7 +6045,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -6052,7 +6056,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -6063,7 +6067,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -6074,7 +6078,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -6087,7 +6091,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>1</v>
+        <v>1713</v>
       </c>
       <c r="B32" t="s">
         <v>12</v>
@@ -6096,7 +6100,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -6107,7 +6111,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -6118,7 +6122,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -6129,7 +6133,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -6140,7 +6144,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -6151,7 +6155,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -6164,7 +6168,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>1</v>
+        <v>1713</v>
       </c>
       <c r="B39" t="s">
         <v>19</v>
@@ -6173,7 +6177,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -6184,7 +6188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -6195,7 +6199,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -6206,7 +6210,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -6217,7 +6221,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -6230,7 +6234,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>1</v>
+        <v>1713</v>
       </c>
       <c r="B45" t="s">
         <v>17</v>
@@ -6239,7 +6243,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>2</v>
       </c>
@@ -6250,7 +6254,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>3</v>
       </c>
@@ -6261,7 +6265,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -6272,7 +6276,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -6283,7 +6287,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -6296,7 +6300,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>1</v>
+        <v>1713</v>
       </c>
       <c r="B51" t="s">
         <v>15</v>
@@ -6305,7 +6309,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>2</v>
       </c>
@@ -6316,7 +6320,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -6327,7 +6331,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -6338,7 +6342,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -6349,7 +6353,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -6360,7 +6364,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -6373,7 +6377,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>1</v>
+        <v>1713</v>
       </c>
       <c r="B58" t="s">
         <v>13</v>
@@ -6382,7 +6386,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>2</v>
       </c>
@@ -6393,7 +6397,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>3</v>
       </c>
@@ -6404,7 +6408,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -6415,7 +6419,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>6</v>
       </c>
@@ -6426,7 +6430,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>7</v>
       </c>
@@ -6439,6 +6443,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:C63" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Profession Plan (Commercial)"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A12:C63">
       <sortCondition ref="A1:A63"/>
     </sortState>

</xml_diff>